<commit_message>
Upload DC and ESP data
</commit_message>
<xml_diff>
--- a/LEM12/RC/data.xlsx
+++ b/LEM12/RC/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinplanck/Desktop/Physics/Physics Lab III/LEM12/RC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C4267-CEF0-6945-B281-1DF065C7173C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71222F47-3EF7-0A42-A55A-ED685AAE2741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15960" activeTab="1" xr2:uid="{20130595-4FA6-AB49-A596-623921EF616F}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{20130595-4FA6-AB49-A596-623921EF616F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,6 +75,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,8 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +433,7 @@
   <dimension ref="A2:P26"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1567,371 +1577,771 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B287B39-9381-1643-80C9-FC7DE0C2FF56}">
-  <dimension ref="A2:E21"/>
+  <dimension ref="A2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>99.9</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
+      <c r="C2" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <f>C2*SQRT((D2/B2)^2 + (1/9.5)^2)</f>
         <v>0.15305558278716258</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>99.9</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="4">
+        <v>9</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <f>9/9</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.15305558278716258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>499</v>
-      </c>
-      <c r="B3">
+        <v>299</v>
+      </c>
+      <c r="B3" s="4">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E21" si="0">C3*SQRT((D3/B3)^2 + (1/9.5)^2)</f>
+      <c r="C3" s="1">
+        <f>B3/9</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f>C3*SQRT((D3/B3)^2 + (1/9.5)^2)</f>
         <v>0.15305558278716258</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>299</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>9</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <f>L3/9</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.15305558278716258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>820</v>
       </c>
-      <c r="B4">
-        <v>8.5</v>
-      </c>
-      <c r="C4">
-        <v>0.94444444444444442</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0.14909413782435044</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C21" si="0">B4/9</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f>C4*SQRT((D4/B4)^2 + (1/9.5)^2)</f>
+        <v>0.14526014442542948</v>
+      </c>
+      <c r="J4">
+        <v>820</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>8</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <f>L4/9</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.14526014442542948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1209</v>
       </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>0.14526014442542948</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f>C5*SQRT((D5/B5)^2 + (1/9.5)^2)</f>
+        <v>0.14156395832643515</v>
+      </c>
+      <c r="J5">
+        <v>1209</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <f>L5/9</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.14156395832643515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>1398</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f>C6*SQRT((D6/B6)^2 + (1/9.5)^2)</f>
+        <v>0.13801665171001107</v>
+      </c>
+      <c r="J6">
+        <v>1398</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>7</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="1">
+        <f>L6/9</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.13801665171001107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1750</v>
       </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>0.77777777777777768</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.13801665171001104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1398</v>
-      </c>
-      <c r="B7">
-        <v>7.5</v>
-      </c>
-      <c r="C7">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0.14156395832643515</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f>C7*SQRT((D7/B7)^2 + (1/9.5)^2)</f>
+        <v>0.13462999337100981</v>
+      </c>
+      <c r="J7">
+        <v>1750</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="1">
+        <f>L7/9</f>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.13462999337100981</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2000</v>
       </c>
-      <c r="B8">
-        <v>6.5</v>
-      </c>
-      <c r="C8">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0.13462999337100981</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f>C8*SQRT((D8/B8)^2 + (1/9.5)^2)</f>
+        <v>0.13141640382598965</v>
+      </c>
+      <c r="J8">
+        <v>2000</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>6</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <f>L8/9</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.13141640382598965</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2260</v>
       </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0.13141640382598965</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f>C9*SQRT((D9/B9)^2 + (1/9.5)^2)</f>
+        <v>0.12838887953274944</v>
+      </c>
+      <c r="J9">
+        <v>2260</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <f>L9/9</f>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.12838887953274944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2760</v>
       </c>
-      <c r="B10">
-        <v>5.5</v>
-      </c>
-      <c r="C10">
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0.12838887953274941</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f>C10*SQRT((D10/B10)^2 + (1/9.5)^2)</f>
+        <v>0.12556088043031516</v>
+      </c>
+      <c r="J10">
+        <v>2760</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <f>L10/9</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.12556088043031516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3070</v>
       </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>0.12556088043031516</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f>C11*SQRT((D11/B11)^2 + (1/9.5)^2)</f>
+        <v>0.12294617568203882</v>
+      </c>
+      <c r="J11">
+        <v>3070</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <f>L11/9</f>
+        <v>0.5</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.12294617568203882</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3420</v>
       </c>
-      <c r="B12">
-        <v>4.5</v>
-      </c>
-      <c r="C12">
-        <v>0.5</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0.12294617568203882</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f>C12*SQRT((D12/B12)^2 + (1/9.5)^2)</f>
+        <v>0.12055864402390819</v>
+      </c>
+      <c r="J12">
+        <v>3420</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <f>L12/9</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0.12055864402390819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4225</v>
       </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>0.12055864402390819</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f>C13*SQRT((D13/B13)^2 + (1/9.5)^2)</f>
+        <v>0.11841202766851805</v>
+      </c>
+      <c r="J13">
+        <v>4225</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <f>L13/9</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0.11841202766851805</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4750</v>
       </c>
-      <c r="B14">
-        <v>3.5</v>
-      </c>
-      <c r="C14">
-        <v>0.38888888888888884</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0.11841202766851804</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f>C14*SQRT((D14/B14)^2 + (1/9.5)^2)</f>
+        <v>0.11651964236942265</v>
+      </c>
+      <c r="J14">
+        <v>4750</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" s="4">
+        <v>3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1">
+        <f>L14/9</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0.11651964236942265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6400</v>
       </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>0.11651964236942265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f>C15*SQRT((D15/B15)^2 + (1/9.5)^2)</f>
+        <v>0.11489405090285675</v>
+      </c>
+      <c r="J15">
+        <v>6400</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <f>L15/9</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0.11489405090285675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7830</v>
       </c>
-      <c r="B16">
-        <v>2.5</v>
-      </c>
-      <c r="C16">
-        <v>0.27777777777777779</v>
-      </c>
-      <c r="D16">
-        <v>0.4</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>5.3200306037633503E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E16" s="2">
+        <f>C16*SQRT((D16/B16)^2 + (1/9.5)^2)</f>
+        <v>5.0224352172126056E-2</v>
+      </c>
+      <c r="J16">
+        <v>7830</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N16" s="2">
+        <f>L16/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="O16" s="2">
+        <v>5.0224352172126056E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9800</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="D17">
-        <v>0.4</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>5.0224352172126056E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="2">
+        <f>C17*SQRT((D17/B17)^2 + (1/9.5)^2)</f>
+        <v>4.7781750212433902E-2</v>
+      </c>
+      <c r="J17">
+        <v>9800</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N17" s="2">
+        <f>L17/9</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="O17" s="2">
+        <v>4.7781750212433902E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>13960</v>
       </c>
-      <c r="B18">
-        <v>1.5</v>
-      </c>
-      <c r="C18">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D18">
-        <v>0.4</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>4.7781750212433902E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E18" s="2">
+        <f>C18*SQRT((D18/B18)^2 + (1/9.5)^2)</f>
+        <v>4.5957620361142697E-2</v>
+      </c>
+      <c r="J18">
+        <v>13960</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N18" s="2">
+        <f>L18/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="O18" s="2">
+        <v>4.5957620361142697E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20640</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="D19">
-        <v>0.4</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>4.5957620361142697E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" ref="E19:E21" si="1">C19*SQRT((D19/B19)^2 + (1/9.5)^2)</f>
+        <v>4.4827527243828776E-2</v>
+      </c>
+      <c r="J19">
+        <v>20640</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N19" s="2">
+        <f>L19/9</f>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="O19" s="2">
+        <v>4.4827527243828776E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>47600</v>
       </c>
-      <c r="B20">
-        <v>0.4</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
         <v>4.4444444444444446E-2</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0.2</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
         <v>2.2709342501693097E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>47600</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N20" s="2">
+        <f>L20/9</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="O20" s="2">
+        <v>2.2709342501693097E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>210000</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>0.1</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
+        <f t="shared" si="0"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>0.04</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E21" s="3">
+        <f t="shared" si="1"/>
+        <v>4.5957620361142693E-3</v>
+      </c>
+      <c r="J21">
+        <v>210000</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="N21" s="3">
+        <f>L21/9</f>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="O21" s="3">
         <v>4.5957620361142693E-3</v>
       </c>
     </row>
@@ -1942,15 +2352,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E70424-7D58-2346-981F-7FFEB3E21587}">
-  <dimension ref="A2:E21"/>
+  <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E21"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>47</v>
       </c>
@@ -1967,8 +2377,27 @@
         <f>C2*SQRT((D2/B2)^2 + (1/9.5)^2)</f>
         <v>1.0757056974486204E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>47</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="N2" s="2">
+        <v>2.1052631578947368E-2</v>
+      </c>
+      <c r="O2" s="2">
+        <f>M2*SQRT((N2/L2)^2 + (1/9.5)^2)</f>
+        <v>1.4886458551295736E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>100</v>
       </c>
@@ -1985,8 +2414,27 @@
         <f t="shared" ref="E3:E21" si="0">C3*SQRT((D3/B3)^2 + (1/9.5)^2)</f>
         <v>2.1769399118436013E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O21" si="1">M3*SQRT((N3/L3)^2 + (1/9.5)^2)</f>
+        <v>2.9772917102591473E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>159.9</v>
       </c>
@@ -2003,8 +2451,27 @@
         <f t="shared" si="0"/>
         <v>2.2250510391161445E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>159.9</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>6.8421052631578952E-2</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9772917102591473E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>200</v>
       </c>
@@ -2021,8 +2488,27 @@
         <f t="shared" si="0"/>
         <v>2.3790482607849182E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>200</v>
+      </c>
+      <c r="K5">
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9772917102591473E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>280</v>
       </c>
@@ -2039,8 +2525,27 @@
         <f t="shared" si="0"/>
         <v>4.5266921253884748E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>280</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.15789473684210525</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>390</v>
       </c>
@@ -2057,8 +2562,27 @@
         <f t="shared" si="0"/>
         <v>4.7580965215698365E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>390</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>508</v>
       </c>
@@ -2075,8 +2599,27 @@
         <f t="shared" si="0"/>
         <v>5.0400289930389627E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>508</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>610</v>
       </c>
@@ -2093,8 +2636,27 @@
         <f t="shared" si="0"/>
         <v>5.3645289471070154E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>610</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>3</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>730</v>
       </c>
@@ -2111,8 +2673,27 @@
         <f t="shared" si="0"/>
         <v>0.11217981568596445</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>730</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>825</v>
       </c>
@@ -2129,8 +2710,27 @@
         <f t="shared" si="0"/>
         <v>0.11421345223317618</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>825</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>970</v>
       </c>
@@ -2147,8 +2747,27 @@
         <f t="shared" si="0"/>
         <v>0.11647532433035256</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>970</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.47368421052631576</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1130</v>
       </c>
@@ -2165,8 +2784,27 @@
         <f t="shared" si="0"/>
         <v>0.11895241303924592</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>1130</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4">
+        <v>5</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1360</v>
       </c>
@@ -2183,8 +2821,27 @@
         <f t="shared" si="0"/>
         <v>0.12163157008365735</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>1360</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0.57894736842105265</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1515</v>
       </c>
@@ -2201,8 +2858,27 @@
         <f t="shared" si="0"/>
         <v>0.12449975099304283</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>1515</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>6</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1732</v>
       </c>
@@ -2219,8 +2895,27 @@
         <f t="shared" si="0"/>
         <v>0.12754420424621982</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>1732</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.68421052631578949</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2580</v>
       </c>
@@ -2237,8 +2932,27 @@
         <f t="shared" si="0"/>
         <v>0.13411322367767539</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>2580</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0.78947368421052633</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4040</v>
       </c>
@@ -2255,8 +2969,27 @@
         <f t="shared" si="0"/>
         <v>0.1412470779388583</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>4040</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0.89473684210526316</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5300</v>
       </c>
@@ -2273,8 +3006,27 @@
         <f t="shared" si="0"/>
         <v>0.14691889868339189</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>5300</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" s="4">
+        <v>9.25</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.97368421052631582</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20000</v>
       </c>
@@ -2291,8 +3043,27 @@
         <f t="shared" si="0"/>
         <v>0.14886458551295736</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>20000</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50000</v>
       </c>
@@ -2307,6 +3078,25 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
+        <v>0.14886458551295736</v>
+      </c>
+      <c r="J21">
+        <v>50000</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="M21" s="4">
+        <v>1</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="1"/>
         <v>0.14886458551295736</v>
       </c>
     </row>
@@ -2317,15 +3107,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F556431-9538-944A-B3C8-C679AC4DF845}">
-  <dimension ref="A2:E21"/>
+  <dimension ref="A2:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11.2</v>
       </c>
@@ -2342,8 +3132,27 @@
         <f>C2*SQRT((D2/B2)^2 + (1/9.5)^2)</f>
         <v>2.1234091852339945E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>11.2</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N2" s="2">
+        <v>2.6315789473684209E-2</v>
+      </c>
+      <c r="O2" s="2">
+        <f>M2*SQRT((N2/L2)^2 + (1/9.5)^2)</f>
+        <v>2.9772917102591473E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>21</v>
       </c>
@@ -2360,8 +3169,27 @@
         <f t="shared" ref="E3:E21" si="0">C3*SQRT((D3/B3)^2 + (1/9.5)^2)</f>
         <v>2.1769399118436013E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ref="O3:O21" si="1">M3*SQRT((N3/L3)^2 + (1/9.5)^2)</f>
+        <v>2.9772917102591473E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>45</v>
       </c>
@@ -2378,8 +3206,27 @@
         <f t="shared" si="0"/>
         <v>2.3790482607849182E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="1"/>
+        <v>2.9772917102591473E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>82.1</v>
       </c>
@@ -2396,8 +3243,27 @@
         <f t="shared" si="0"/>
         <v>4.5685380893270476E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>82.1</v>
+      </c>
+      <c r="K5">
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.16842105263157894</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>101</v>
       </c>
@@ -2414,8 +3280,27 @@
         <f t="shared" si="0"/>
         <v>4.7580965215698365E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>101</v>
+      </c>
+      <c r="K6">
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>151.6</v>
       </c>
@@ -2432,8 +3317,27 @@
         <f t="shared" si="0"/>
         <v>5.1017681698487929E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>151.6</v>
+      </c>
+      <c r="K7">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.27368421052631581</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>182.9</v>
       </c>
@@ -2450,8 +3354,27 @@
         <f t="shared" si="0"/>
         <v>5.3645289471070154E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>182.9</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>233</v>
       </c>
@@ -2468,8 +3391,27 @@
         <f t="shared" si="0"/>
         <v>5.504594946647854E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>233</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.33684210526315789</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>330</v>
       </c>
@@ -2486,8 +3428,27 @@
         <f t="shared" si="0"/>
         <v>0.11421345223317618</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>330</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
+        <v>4</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>830</v>
       </c>
@@ -2504,8 +3465,27 @@
         <f t="shared" si="0"/>
         <v>0.11531666646259638</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>830</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4.25</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0.44736842105263158</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1022</v>
       </c>
@@ -2522,8 +3502,27 @@
         <f t="shared" si="0"/>
         <v>0.11531666646259638</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>1022</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4.25</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0.44736842105263158</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2210</v>
       </c>
@@ -2540,8 +3539,27 @@
         <f t="shared" si="0"/>
         <v>0.11421345223317618</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>2210</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4">
+        <v>4</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3430</v>
       </c>
@@ -2558,8 +3576,27 @@
         <f t="shared" si="0"/>
         <v>0.11217981568596445</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>3430</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4610</v>
       </c>
@@ -2576,8 +3613,27 @@
         <f t="shared" si="0"/>
         <v>0.11038702961313725</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>4610</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15" s="4">
+        <v>3</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6150</v>
       </c>
@@ -2594,8 +3650,27 @@
         <f t="shared" si="0"/>
         <v>0.10884699559218007</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>6150</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8380</v>
       </c>
@@ -2612,8 +3687,27 @@
         <f t="shared" si="0"/>
         <v>0.10757056974486204</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>8380</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17" s="4">
+        <v>2</v>
+      </c>
+      <c r="M17" s="4">
+        <v>1</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14886458551295736</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>11430</v>
       </c>
@@ -2630,8 +3724,27 @@
         <f t="shared" si="0"/>
         <v>4.5266921253884748E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>11430</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.15789473684210525</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20420</v>
       </c>
@@ -2648,8 +3761,27 @@
         <f t="shared" si="0"/>
         <v>4.3538798236872026E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>20420</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>47700</v>
       </c>
@@ -2666,8 +3798,27 @@
         <f t="shared" si="0"/>
         <v>4.246818370467989E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>47700</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N20" s="2">
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>99400</v>
       </c>
@@ -2683,6 +3834,25 @@
       <c r="E21">
         <f t="shared" si="0"/>
         <v>4.2163540366627027E-2</v>
+      </c>
+      <c r="J21">
+        <v>99400</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="N21" s="2">
+        <v>2.1052631578947368E-2</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9545834205182946E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>